<commit_message>
Added implementation phase contributions
</commit_message>
<xml_diff>
--- a/Gantt project planner.xlsx
+++ b/Gantt project planner.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="193" documentId="8_{0FB9448C-D13E-40D1-A725-216C815851DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1987CED1-AA3A-4298-8D94-9EBEFD9DE868}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3B7258-AFB7-4F47-955C-6D8D2B76236E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3600" yWindow="2985" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="55">
   <si>
     <t xml:space="preserve">Blackjack project Tasks </t>
   </si>
@@ -207,6 +207,9 @@
   </si>
   <si>
     <t>Implementation phase contribution</t>
+  </si>
+  <si>
+    <t>Client, Server, Message, GUI, Panels</t>
   </si>
 </sst>
 </file>
@@ -1653,10 +1656,6 @@
 </FeaturePropertyBags>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{050161F6-637A-4AAB-AA3F-A284F6562292}" name="Table2" displayName="Table2" ref="A2:F8" totalsRowShown="0">
   <autoFilter ref="A2:F8" xr:uid="{050161F6-637A-4AAB-AA3F-A284F6562292}"/>
@@ -1929,27 +1928,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22311CCC-0325-4A31-9EFD-58D1C23F0A25}">
   <dimension ref="A2:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E56" sqref="E56"/>
+    <sheetView tabSelected="1" topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.08203125" customWidth="1"/>
-    <col min="2" max="2" width="29.6640625" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" customWidth="1"/>
-    <col min="7" max="7" width="8.58203125" customWidth="1"/>
+    <col min="1" max="1" width="36.125" customWidth="1"/>
+    <col min="2" max="2" width="29.625" customWidth="1"/>
+    <col min="3" max="3" width="45.625" customWidth="1"/>
+    <col min="4" max="4" width="33.625" customWidth="1"/>
+    <col min="5" max="5" width="19.875" customWidth="1"/>
+    <col min="6" max="6" width="21.375" customWidth="1"/>
+    <col min="7" max="7" width="8.625" customWidth="1"/>
     <col min="8" max="10" width="9.5" customWidth="1"/>
-    <col min="11" max="11" width="9.6640625" customWidth="1"/>
+    <col min="11" max="11" width="9.625" customWidth="1"/>
     <col min="12" max="12" width="9.5" customWidth="1"/>
-    <col min="13" max="13" width="9.6640625" customWidth="1"/>
+    <col min="13" max="13" width="9.625" customWidth="1"/>
     <col min="14" max="14" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1969,7 +1968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -1989,7 +1988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2009,7 +2008,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2029,7 +2028,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2045,7 +2044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2061,7 +2060,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2075,46 +2074,46 @@
       <c r="E8" s="4"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -2128,7 +2127,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -2142,7 +2141,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -2156,7 +2155,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -2170,7 +2169,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -2184,7 +2183,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -2198,7 +2197,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -2212,7 +2211,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -2226,7 +2225,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2240,7 +2239,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2254,7 +2253,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2268,7 +2267,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -2282,11 +2281,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B40" s="1"/>
       <c r="C40" s="3"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>35</v>
       </c>
@@ -2306,7 +2305,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>18</v>
       </c>
@@ -2317,7 +2316,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>22</v>
       </c>
@@ -2328,7 +2327,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>26</v>
       </c>
@@ -2339,7 +2338,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>30</v>
       </c>
@@ -2349,8 +2348,11 @@
       <c r="C49" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D49" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
updated what i worked for test
</commit_message>
<xml_diff>
--- a/Gantt project planner.xlsx
+++ b/Gantt project planner.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{736F8D8E-73DE-4DA7-915A-7528EF397ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5179FBA0-0785-41CB-ACA5-5FDBCFE2C446}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100CF829-359D-4220-8CDC-1EA57187649C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
   <si>
     <t xml:space="preserve">Blackjack project Tasks </t>
   </si>
@@ -232,6 +232,9 @@
   </si>
   <si>
     <t>server (in the start) , player , Penals, testing</t>
+  </si>
+  <si>
+    <t>Added TestRunner and AllTest</t>
   </si>
 </sst>
 </file>
@@ -1944,27 +1947,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22311CCC-0325-4A31-9EFD-58D1C23F0A25}">
   <dimension ref="A2:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.08203125" customWidth="1"/>
-    <col min="2" max="2" width="29.58203125" customWidth="1"/>
-    <col min="3" max="3" width="45.58203125" customWidth="1"/>
-    <col min="4" max="4" width="33.58203125" customWidth="1"/>
-    <col min="5" max="5" width="19.83203125" customWidth="1"/>
-    <col min="6" max="6" width="21.33203125" customWidth="1"/>
-    <col min="7" max="7" width="8.58203125" customWidth="1"/>
+    <col min="1" max="1" width="36.125" customWidth="1"/>
+    <col min="2" max="2" width="29.625" customWidth="1"/>
+    <col min="3" max="3" width="45.625" customWidth="1"/>
+    <col min="4" max="4" width="33.625" customWidth="1"/>
+    <col min="5" max="5" width="39" customWidth="1"/>
+    <col min="6" max="6" width="21.375" customWidth="1"/>
+    <col min="7" max="7" width="8.625" customWidth="1"/>
     <col min="8" max="10" width="9.5" customWidth="1"/>
-    <col min="11" max="11" width="9.58203125" customWidth="1"/>
+    <col min="11" max="11" width="9.625" customWidth="1"/>
     <col min="12" max="12" width="9.5" customWidth="1"/>
-    <col min="13" max="13" width="9.58203125" customWidth="1"/>
+    <col min="13" max="13" width="9.625" customWidth="1"/>
     <col min="14" max="14" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1984,7 +1987,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -2004,7 +2007,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -2024,7 +2027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -2044,7 +2047,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -2064,7 +2067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -2078,7 +2081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -2088,46 +2091,46 @@
       <c r="E8" s="4"/>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B27" s="3"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>12</v>
       </c>
@@ -2141,7 +2144,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>16</v>
       </c>
@@ -2155,7 +2158,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>20</v>
       </c>
@@ -2169,7 +2172,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>24</v>
       </c>
@@ -2183,7 +2186,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -2197,7 +2200,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -2211,7 +2214,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -2225,7 +2228,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -2239,7 +2242,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -2253,7 +2256,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -2267,7 +2270,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -2281,7 +2284,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -2295,7 +2298,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>55</v>
       </c>
@@ -2309,7 +2312,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>55</v>
       </c>
@@ -2323,7 +2326,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>58</v>
       </c>
@@ -2337,7 +2340,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>55</v>
       </c>
@@ -2351,7 +2354,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>58</v>
       </c>
@@ -2365,7 +2368,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>55</v>
       </c>
@@ -2379,7 +2382,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>55</v>
       </c>
@@ -2393,7 +2396,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>55</v>
       </c>
@@ -2407,7 +2410,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>58</v>
       </c>
@@ -2421,13 +2424,13 @@
         <v>180</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B49" s="1"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B50" s="1"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>35</v>
       </c>
@@ -2447,7 +2450,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>18</v>
       </c>
@@ -2461,7 +2464,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>22</v>
       </c>
@@ -2472,7 +2475,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>26</v>
       </c>
@@ -2483,7 +2486,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>30</v>
       </c>
@@ -2497,7 +2500,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>33</v>
       </c>
@@ -2509,6 +2512,9 @@
       </c>
       <c r="D57" t="s">
         <v>54</v>
+      </c>
+      <c r="E57" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edited and uploaded test plan
</commit_message>
<xml_diff>
--- a/Gantt project planner.xlsx
+++ b/Gantt project planner.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{100CF829-359D-4220-8CDC-1EA57187649C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276AF8D4-34F5-47F0-86A7-085EA56A2AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
   <si>
     <t xml:space="preserve">Blackjack project Tasks </t>
   </si>
@@ -231,10 +231,22 @@
     <t>10:00 ~ 1:00</t>
   </si>
   <si>
-    <t>server (in the start) , player , Penals, testing</t>
-  </si>
-  <si>
     <t>Added TestRunner and AllTest</t>
+  </si>
+  <si>
+    <t>Game, Table, Lobby, Player, Dealer</t>
+  </si>
+  <si>
+    <t>Hand, Message, Shoe Test</t>
+  </si>
+  <si>
+    <t>Table, Lobby, Player, Dealer, Message</t>
+  </si>
+  <si>
+    <t>Login, Hand, Server, Client, Deck, Card</t>
+  </si>
+  <si>
+    <t>Server (in the start) , player , Penals, testing</t>
   </si>
 </sst>
 </file>
@@ -1947,16 +1959,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22311CCC-0325-4A31-9EFD-58D1C23F0A25}">
   <dimension ref="A2:F57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="36.125" customWidth="1"/>
     <col min="2" max="2" width="29.625" customWidth="1"/>
-    <col min="3" max="3" width="45.625" customWidth="1"/>
-    <col min="4" max="4" width="33.625" customWidth="1"/>
+    <col min="3" max="3" width="53.75" customWidth="1"/>
+    <col min="4" max="4" width="46.625" customWidth="1"/>
     <col min="5" max="5" width="39" customWidth="1"/>
     <col min="6" max="6" width="21.375" customWidth="1"/>
     <col min="7" max="7" width="8.625" customWidth="1"/>
@@ -2461,7 +2473,7 @@
         <v>45</v>
       </c>
       <c r="D53" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2474,6 +2486,12 @@
       <c r="C54" t="s">
         <v>46</v>
       </c>
+      <c r="D54" t="s">
+        <v>66</v>
+      </c>
+      <c r="E54" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
@@ -2485,6 +2503,12 @@
       <c r="C55" t="s">
         <v>47</v>
       </c>
+      <c r="D55" t="s">
+        <v>69</v>
+      </c>
+      <c r="E55" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
@@ -2514,7 +2538,7 @@
         <v>54</v>
       </c>
       <c r="E57" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added who worked on what
</commit_message>
<xml_diff>
--- a/Gantt project planner.xlsx
+++ b/Gantt project planner.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276AF8D4-34F5-47F0-86A7-085EA56A2AA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C827050-EA8F-4A54-830E-EB0EAC80942C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
   <si>
     <t xml:space="preserve">Blackjack project Tasks </t>
   </si>
@@ -240,13 +240,16 @@
     <t>Hand, Message, Shoe Test</t>
   </si>
   <si>
-    <t>Table, Lobby, Player, Dealer, Message</t>
-  </si>
-  <si>
-    <t>Login, Hand, Server, Client, Deck, Card</t>
-  </si>
-  <si>
     <t>Server (in the start) , player , Penals, testing</t>
+  </si>
+  <si>
+    <t>Client, Card, Server, Message, GUI, Panels</t>
+  </si>
+  <si>
+    <t>Login, Hand, Server, Client, Deck</t>
+  </si>
+  <si>
+    <t>Table, Lobby, Player, Dealer</t>
   </si>
 </sst>
 </file>
@@ -1960,7 +1963,7 @@
   <dimension ref="A2:F57"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A29" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2473,7 +2476,7 @@
         <v>45</v>
       </c>
       <c r="D53" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -2490,7 +2493,7 @@
         <v>66</v>
       </c>
       <c r="E54" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -2504,7 +2507,7 @@
         <v>47</v>
       </c>
       <c r="D55" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E55" t="s">
         <v>67</v>
@@ -2521,7 +2524,7 @@
         <v>48</v>
       </c>
       <c r="D56" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>